<commit_message>
Added Trevor, Alec, and Adam to the mix
</commit_message>
<xml_diff>
--- a/CMQA/Organization/RCL-B-CMQA1 Spring 2014 Rascal Personnel Budget.xlsx
+++ b/CMQA/Organization/RCL-B-CMQA1 Spring 2014 Rascal Personnel Budget.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="148">
   <si>
     <t>Lead</t>
   </si>
@@ -35,9 +35,6 @@
     <t>CDH</t>
   </si>
   <si>
-    <t>Communication</t>
-  </si>
-  <si>
     <t>Payload</t>
   </si>
   <si>
@@ -383,9 +380,6 @@
     <t>Joseph Mayer</t>
   </si>
   <si>
-    <t>Alex Howard</t>
-  </si>
-  <si>
     <t>Peter Rackovan</t>
   </si>
   <si>
@@ -441,13 +435,43 @@
   </si>
   <si>
     <t>dvehab@slu.edu</t>
+  </si>
+  <si>
+    <t>Casey Smith</t>
+  </si>
+  <si>
+    <t>Adam Oneill</t>
+  </si>
+  <si>
+    <t>Oneill</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>oneilla@slu.edu</t>
+  </si>
+  <si>
+    <t>nbossart@slu.edu</t>
+  </si>
+  <si>
+    <t>jmayer16@slu.edu</t>
+  </si>
+  <si>
+    <t>sarber@slu.edu</t>
+  </si>
+  <si>
+    <t>rurberge@slu.edu</t>
+  </si>
+  <si>
+    <t>Alec Herzog</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -501,6 +525,11 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -738,7 +767,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
@@ -795,6 +824,8 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -1135,7 +1166,7 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Master Contact Info'!$A$34:$A$38</c:f>
+              <c:f>'Master Contact Info'!$A$35:$A$39</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1158,12 +1189,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Master Contact Info'!$B$34:$B$38</c:f>
+              <c:f>'Master Contact Info'!$B$35:$B$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3</c:v>
@@ -1250,9 +1281,9 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Master Contact Info'!$A$41:$A$46</c:f>
+              <c:f>'Master Contact Info'!$A$42:$A$48</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>Command and Data Handling</c:v>
                 </c:pt>
@@ -1269,6 +1300,9 @@
                   <c:v>Power</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>Attitude Determination and Control</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>Propulsion</c:v>
                 </c:pt>
               </c:strCache>
@@ -1276,10 +1310,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Master Contact Info'!$B$41:$B$46</c:f>
+              <c:f>'Master Contact Info'!$B$42:$B$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1287,7 +1321,7 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2</c:v>
@@ -1296,7 +1330,10 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1434,8 +1471,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H25" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" headerRowCellStyle="Check Cell">
-  <autoFilter ref="A1:H25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H26" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" headerRowCellStyle="Check Cell">
+  <autoFilter ref="A1:H26"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Last Name" dataDxfId="7"/>
     <tableColumn id="2" name="First Name" dataDxfId="6"/>
@@ -1741,7 +1778,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" thickTop="1" thickBottom="1"/>
@@ -1763,28 +1800,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="18" t="s">
-        <v>6</v>
-      </c>
       <c r="H1" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J1" s="4"/>
     </row>
@@ -1793,28 +1830,26 @@
         <v>0</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E2" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>120</v>
-      </c>
+      <c r="G2" s="8"/>
       <c r="H2" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:10" thickTop="1" thickBot="1">
@@ -1822,26 +1857,24 @@
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>121</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="G3" s="8"/>
       <c r="H3" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:10" thickTop="1" thickBot="1">
@@ -1852,42 +1885,44 @@
         <v>3</v>
       </c>
       <c r="D6" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="F6" s="29" t="s">
+      <c r="G6" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="29" t="s">
-        <v>6</v>
-      </c>
       <c r="H6" s="29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I6" s="29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:10" thickTop="1" thickBot="1">
       <c r="B7" s="28" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="C7" s="28"/>
       <c r="D7" s="28"/>
       <c r="E7" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="F7" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="F7" s="28" t="s">
+      <c r="G7" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="I7" s="28" t="s">
         <v>126</v>
-      </c>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28" t="s">
-        <v>127</v>
-      </c>
-      <c r="I7" s="28" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:10" thickTop="1" thickBot="1">
@@ -1897,41 +1932,47 @@
       <c r="C8" s="28"/>
       <c r="D8" s="28"/>
       <c r="E8" s="28" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F8" s="28"/>
       <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
+      <c r="H8" s="28" t="s">
+        <v>139</v>
+      </c>
       <c r="I8" s="28" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:10" thickTop="1" thickBot="1">
-      <c r="B9" s="28" t="s">
-        <v>99</v>
+      <c r="B9" t="s">
+        <v>121</v>
       </c>
       <c r="C9" s="28"/>
       <c r="D9" s="28"/>
       <c r="E9" s="28" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F9" s="28"/>
       <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
+      <c r="H9" s="28" t="s">
+        <v>147</v>
+      </c>
       <c r="I9" s="28" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:10" thickTop="1" thickBot="1">
       <c r="B10" s="28"/>
       <c r="C10" s="28"/>
       <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
+      <c r="E10" s="28" t="s">
+        <v>138</v>
+      </c>
       <c r="F10" s="28"/>
       <c r="G10" s="28"/>
       <c r="H10" s="28"/>
       <c r="I10" s="28" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:10" thickTop="1" thickBot="1">
@@ -1943,7 +1984,7 @@
       <c r="G11" s="28"/>
       <c r="H11" s="28"/>
       <c r="I11" s="28" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:10" thickTop="1" thickBot="1">
@@ -1955,7 +1996,7 @@
       <c r="G12" s="28"/>
       <c r="H12" s="28"/>
       <c r="I12" s="28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:10" thickTop="1" thickBot="1">
@@ -1984,15 +2025,15 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
@@ -2004,199 +2045,203 @@
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="A1" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>26</v>
-      </c>
       <c r="D1" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="F1" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="G1" s="16" t="s">
+      <c r="H1" s="26" t="s">
         <v>11</v>
-      </c>
-      <c r="H1" s="26" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="A2" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="C2" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="G2" s="32" t="s">
         <v>79</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" s="31" t="s">
-        <v>104</v>
-      </c>
-      <c r="G2" s="32" t="s">
-        <v>80</v>
       </c>
       <c r="H2" s="37"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickTop="1">
       <c r="A3" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="23" t="s">
-        <v>46</v>
-      </c>
       <c r="C3" s="23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F3" s="31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H3" s="24"/>
       <c r="I3" s="9"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F4" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="34"/>
+        <v>4</v>
+      </c>
+      <c r="G4" s="47" t="s">
+        <v>143</v>
+      </c>
       <c r="H4" s="13"/>
       <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="G5" s="34" t="s">
         <v>60</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="F5" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="G5" s="34" t="s">
-        <v>61</v>
       </c>
       <c r="H5" s="24"/>
       <c r="I5" s="9"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="C6" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="10" t="s">
+      <c r="E6" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="G6" s="34" t="s">
         <v>83</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="G6" s="34" t="s">
-        <v>84</v>
       </c>
       <c r="H6" s="13"/>
       <c r="I6" s="9"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F7" s="31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G7" s="34" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H7" s="27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I7" s="12"/>
       <c r="J7" s="11"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="C8" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="G8" s="34" t="s">
         <v>68</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="F8" s="31"/>
-      <c r="G8" s="34" t="s">
-        <v>69</v>
       </c>
       <c r="H8" s="24"/>
       <c r="I8" s="12"/>
@@ -2204,25 +2249,25 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="C9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="34" t="s">
         <v>76</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" s="31" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="34" t="s">
-        <v>77</v>
       </c>
       <c r="H9" s="13"/>
       <c r="I9" s="12"/>
@@ -2230,25 +2275,25 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="C10" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="G10" s="32" t="s">
         <v>63</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="F10" s="31" t="s">
-        <v>104</v>
-      </c>
-      <c r="G10" s="32" t="s">
-        <v>64</v>
       </c>
       <c r="H10" s="24"/>
       <c r="I10" s="12"/>
@@ -2256,25 +2301,25 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="C11" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="G11" s="32" t="s">
         <v>102</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="F11" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="G11" s="32" t="s">
-        <v>103</v>
       </c>
       <c r="H11" s="13"/>
       <c r="I11" s="12"/>
@@ -2282,49 +2327,51 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="14" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F12" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="G12" s="32"/>
+        <v>4</v>
+      </c>
+      <c r="G12" s="47" t="s">
+        <v>144</v>
+      </c>
       <c r="H12" s="13"/>
       <c r="I12" s="12"/>
       <c r="J12" s="11"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="C13" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="23" t="s">
+      <c r="E13" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="G13" s="34" t="s">
         <v>58</v>
-      </c>
-      <c r="E13" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="F13" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="G13" s="34" t="s">
-        <v>59</v>
       </c>
       <c r="H13" s="24"/>
       <c r="I13" s="12"/>
@@ -2332,81 +2379,81 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F14" s="31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G14" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="27" t="s">
         <v>31</v>
-      </c>
-      <c r="H14" s="27" t="s">
-        <v>32</v>
       </c>
       <c r="I14" s="12"/>
       <c r="J14" s="11"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F15" s="31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G15" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" s="27" t="s">
         <v>35</v>
-      </c>
-      <c r="H15" s="27" t="s">
-        <v>36</v>
       </c>
       <c r="I15" s="12"/>
       <c r="J15" s="11"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="14" t="s">
-        <v>113</v>
+        <v>140</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>112</v>
+        <v>141</v>
       </c>
       <c r="C16" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="10" t="s">
-        <v>28</v>
-      </c>
       <c r="E16" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F16" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="G16" s="32" t="s">
-        <v>114</v>
+        <v>104</v>
+      </c>
+      <c r="G16" s="46" t="s">
+        <v>142</v>
       </c>
       <c r="H16" s="13"/>
       <c r="I16" s="12"/>
@@ -2414,232 +2461,256 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="14" t="s">
-        <v>85</v>
+        <v>112</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="C17" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="10" t="s">
-        <v>13</v>
-      </c>
       <c r="E17" s="10" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="F17" s="31" t="s">
-        <v>108</v>
+        <v>70</v>
       </c>
       <c r="G17" s="32" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="H17" s="13"/>
       <c r="I17" s="12"/>
       <c r="J17" s="11"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="24" t="s">
-        <v>47</v>
+      <c r="A18" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="F18" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="G18" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="H18" s="24"/>
-      <c r="I18" s="9"/>
+        <v>107</v>
+      </c>
+      <c r="G18" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="H18" s="13"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="11"/>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="22" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D19" s="23" t="s">
         <v>13</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="F19" s="31" t="s">
-        <v>110</v>
-      </c>
-      <c r="G19" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="H19" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="G19" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="H19" s="24"/>
+      <c r="I19" s="9"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="I19" s="9"/>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>54</v>
-      </c>
       <c r="F20" s="31" t="s">
-        <v>104</v>
-      </c>
-      <c r="G20" s="32"/>
-      <c r="H20" s="13"/>
+        <v>109</v>
+      </c>
+      <c r="G20" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20" s="24" t="s">
+        <v>37</v>
+      </c>
       <c r="I20" s="9"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="14" t="s">
-        <v>16</v>
+        <v>136</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>73</v>
+        <v>114</v>
       </c>
       <c r="C21" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="10" t="s">
-        <v>42</v>
-      </c>
       <c r="E21" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F21" s="31"/>
-      <c r="G21" s="32" t="s">
-        <v>74</v>
+        <v>53</v>
+      </c>
+      <c r="F21" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="G21" s="47" t="s">
+        <v>145</v>
       </c>
       <c r="H21" s="13"/>
       <c r="I21" s="9"/>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="14" t="s">
-        <v>137</v>
+        <v>15</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>136</v>
+        <v>72</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="F22" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="G22" s="32"/>
+        <v>70</v>
+      </c>
+      <c r="G22" s="32" t="s">
+        <v>73</v>
+      </c>
       <c r="H22" s="13"/>
       <c r="I22" s="9"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23" s="47" t="s">
+        <v>146</v>
+      </c>
+      <c r="H23" s="13"/>
+      <c r="I23" s="9"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="B23" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" s="23" t="s">
+      <c r="C24" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="G24" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="H24" s="24"/>
+      <c r="I24" s="9"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F25" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="G25" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="H25" s="13"/>
+      <c r="I25" s="9"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="E23" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="F23" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="G23" s="32" t="s">
-        <v>139</v>
-      </c>
-      <c r="H23" s="24"/>
-      <c r="I23" s="9"/>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F24" s="31"/>
-      <c r="G24" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="H24" s="13"/>
-      <c r="I24" s="9"/>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="19" t="s">
+      <c r="E26" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="D25" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="E25" s="21" t="s">
+      <c r="F26" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="G26" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="F25" s="38" t="s">
-        <v>104</v>
-      </c>
-      <c r="G25" s="39" t="s">
-        <v>55</v>
-      </c>
-      <c r="H25" s="21"/>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="40"/>
-      <c r="B26" s="40"/>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
-      <c r="F26" s="41"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="43"/>
+      <c r="H26" s="21"/>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="40"/>
@@ -2648,16 +2719,12 @@
       <c r="D27" s="40"/>
       <c r="E27" s="40"/>
       <c r="F27" s="41"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="40"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="43"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="44" t="s">
-        <v>92</v>
-      </c>
-      <c r="B28" s="44" t="s">
-        <v>93</v>
-      </c>
+      <c r="A28" s="40"/>
+      <c r="B28" s="40"/>
       <c r="C28" s="40"/>
       <c r="D28" s="40"/>
       <c r="E28" s="40"/>
@@ -2666,12 +2733,11 @@
       <c r="H28" s="40"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" s="23">
-        <f t="array" ref="B29">SUM(IF(C2:C25="AE",1,0))</f>
-        <v>20</v>
+      <c r="A29" s="44" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" s="44" t="s">
+        <v>92</v>
       </c>
       <c r="C29" s="40"/>
       <c r="D29" s="40"/>
@@ -2682,11 +2748,11 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B30" s="23">
-        <f t="array" ref="B30">SUM(IF(C2:C25="EE",1,0))</f>
-        <v>3</v>
+        <f t="array" ref="B30">SUM(IF(C2:C26="AE",1,0))</f>
+        <v>21</v>
       </c>
       <c r="C30" s="40"/>
       <c r="D30" s="40"/>
@@ -2697,10 +2763,11 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="10" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B31" s="23">
-        <v>1</v>
+        <f t="array" ref="B31">SUM(IF(C2:C26="EE",1,0))</f>
+        <v>3</v>
       </c>
       <c r="C31" s="40"/>
       <c r="D31" s="40"/>
@@ -2710,8 +2777,12 @@
       <c r="H31" s="40"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="40"/>
-      <c r="B32" s="40"/>
+      <c r="A32" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="23">
+        <v>1</v>
+      </c>
       <c r="C32" s="40"/>
       <c r="D32" s="40"/>
       <c r="E32" s="40"/>
@@ -2720,12 +2791,8 @@
       <c r="H32" s="40"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="44" t="s">
-        <v>94</v>
-      </c>
-      <c r="B33" s="44" t="s">
-        <v>95</v>
-      </c>
+      <c r="A33" s="40"/>
+      <c r="B33" s="40"/>
       <c r="C33" s="40"/>
       <c r="D33" s="40"/>
       <c r="E33" s="40"/>
@@ -2734,12 +2801,11 @@
       <c r="H33" s="40"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B34" s="23">
-        <f t="array" ref="B34">SUM(IF(D2:D25="Freshman",1,0))</f>
-        <v>7</v>
+      <c r="A34" s="44" t="s">
+        <v>93</v>
+      </c>
+      <c r="B34" s="44" t="s">
+        <v>94</v>
       </c>
       <c r="C34" s="40"/>
       <c r="D34" s="40"/>
@@ -2750,11 +2816,11 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="10" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="B35" s="23">
-        <f t="array" ref="B35">SUM(IF(D2:D25="Sophomore",1,0))</f>
-        <v>3</v>
+        <f t="array" ref="B35">SUM(IF(D2:D26="Freshman",1,0))</f>
+        <v>8</v>
       </c>
       <c r="C35" s="40"/>
       <c r="D35" s="40"/>
@@ -2764,24 +2830,27 @@
       <c r="H35" s="40"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B36" s="1">
-        <f t="array" ref="B36">SUM(IF(D2:D25="Junior",1,0))</f>
-        <v>4</v>
-      </c>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="G36" s="11"/>
+      <c r="A36" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="23">
+        <f t="array" ref="B36">SUM(IF(D2:D26="Sophomore",1,0))</f>
+        <v>3</v>
+      </c>
+      <c r="C36" s="40"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="41"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="40"/>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B37" s="1">
-        <f t="array" ref="B37">SUM(IF(D2:D25="Senior",1,0))</f>
-        <v>8</v>
+        <f t="array" ref="B37">SUM(IF(D2:D26="Junior",1,0))</f>
+        <v>4</v>
       </c>
       <c r="D37" s="11"/>
       <c r="E37" s="11"/>
@@ -2789,78 +2858,78 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
-        <v>83</v>
+        <v>12</v>
       </c>
       <c r="B38" s="1">
-        <f t="array" ref="B38">SUM(IF(D2:D25="Graduate",1,0))</f>
+        <f t="array" ref="B38">SUM(IF(D2:D26="Senior",1,0))</f>
+        <v>8</v>
+      </c>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="G38" s="11"/>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B39" s="1">
+        <f t="array" ref="B39">SUM(IF(D2:D26="Graduate",1,0))</f>
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
-      <c r="A40" s="44" t="s">
+    <row r="41" spans="1:8">
+      <c r="A41" s="44" t="s">
+        <v>95</v>
+      </c>
+      <c r="B41" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="B40" s="44" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
-      <c r="A41" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B41" s="1">
-        <f t="array" ref="B41">SUM(IF(ISNUMBER(SEARCH(A41,$F$2:$F$25)),1,0))</f>
-        <v>1</v>
-      </c>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="G41" s="11"/>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="B42" s="1">
-        <f t="array" ref="B42">SUM(IF(ISNUMBER(SEARCH(A42,$F$2:$F$25)),1,0))</f>
-        <v>9</v>
-      </c>
+        <f t="array" ref="B42">SUM(IF(ISNUMBER(SEARCH(A42,$F$2:$F$26)),1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="G42" s="11"/>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
-        <v>71</v>
+        <v>103</v>
       </c>
       <c r="B43" s="1">
-        <f t="array" ref="B43">SUM(IF(ISNUMBER(SEARCH(A43,$F$2:$F$25)),1,0))</f>
-        <v>5</v>
+        <f t="array" ref="B43">SUM(IF(ISNUMBER(SEARCH(A43,$F$2:$F$26)),1,0))</f>
+        <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="B44" s="1">
-        <f t="array" ref="B44">SUM(IF(ISNUMBER(SEARCH(A44,$F$2:$F$25)),1,0))</f>
-        <v>2</v>
+        <f t="array" ref="B44">SUM(IF(ISNUMBER(SEARCH(A44,$F$2:$F$26)),1,0))</f>
+        <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
-        <v>6</v>
+        <v>86</v>
       </c>
       <c r="B45" s="1">
-        <f t="array" ref="B45">SUM(IF(ISNUMBER(SEARCH(A45,$F$2:$F$25)),1,0))</f>
-        <v>3</v>
-      </c>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="G45" s="11"/>
+        <f t="array" ref="B45">SUM(IF(ISNUMBER(SEARCH(A45,$F$2:$F$26)),1,0))</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
-        <v>105</v>
+        <v>5</v>
       </c>
       <c r="B46" s="1">
-        <f t="array" ref="B46">SUM(IF(ISNUMBER(SEARCH(A46,$F$2:$F$25)),1,0))</f>
+        <f t="array" ref="B46">SUM(IF(ISNUMBER(SEARCH(A46,$F$2:$F$26)),1,0))</f>
         <v>3</v>
       </c>
       <c r="D46" s="11"/>
@@ -2868,38 +2937,66 @@
       <c r="G46" s="11"/>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="45" t="s">
+      <c r="A47" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B47" s="1">
+        <f t="array" ref="B47">SUM(IF(ISNUMBER(SEARCH(A47,$F$2:$F$26)),1,0))</f>
+        <v>6</v>
+      </c>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="G47" s="11"/>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B48" s="1">
+        <f t="array" ref="B48">SUM(IF(ISNUMBER(SEARCH(A48,$F$2:$F$26)),1,0))</f>
         <v>5</v>
       </c>
-      <c r="B47" s="45">
-        <f t="array" ref="B47">SUM(IF(ISNUMBER(SEARCH(A47,$F$2:$F$25)),1,0))</f>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="G48" s="11"/>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49" s="45">
+        <f t="array" ref="B49">SUM(IF(ISNUMBER(SEARCH(A49,$F$2:$F$26)),1,0))</f>
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G3" r:id="rId1"/>
-    <hyperlink ref="G18" r:id="rId2"/>
-    <hyperlink ref="G25" r:id="rId3"/>
+    <hyperlink ref="G19" r:id="rId2"/>
+    <hyperlink ref="G26" r:id="rId3"/>
     <hyperlink ref="G13" r:id="rId4"/>
     <hyperlink ref="G5" r:id="rId5"/>
     <hyperlink ref="G10" r:id="rId6"/>
-    <hyperlink ref="G23" r:id="rId7"/>
+    <hyperlink ref="G24" r:id="rId7"/>
     <hyperlink ref="G8" r:id="rId8"/>
-    <hyperlink ref="G21" r:id="rId9"/>
+    <hyperlink ref="G22" r:id="rId9"/>
     <hyperlink ref="G9" r:id="rId10"/>
     <hyperlink ref="G2" r:id="rId11"/>
     <hyperlink ref="G6" r:id="rId12"/>
-    <hyperlink ref="G17" r:id="rId13"/>
-    <hyperlink ref="G24" r:id="rId14"/>
+    <hyperlink ref="G18" r:id="rId13"/>
+    <hyperlink ref="G25" r:id="rId14"/>
     <hyperlink ref="G11" r:id="rId15"/>
     <hyperlink ref="G7" r:id="rId16"/>
-    <hyperlink ref="G16" r:id="rId17"/>
+    <hyperlink ref="G17" r:id="rId17"/>
+    <hyperlink ref="G4" r:id="rId18" display="mailto:nbossart@slu.edu"/>
+    <hyperlink ref="G12" r:id="rId19" display="mailto:jmayer16@slu.edu"/>
+    <hyperlink ref="G21" r:id="rId20" display="mailto:sarber@slu.edu"/>
+    <hyperlink ref="G23" r:id="rId21" display="mailto:rurberge@slu.edu"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="78" orientation="landscape" r:id="rId18"/>
+  <pageSetup scale="78" orientation="landscape" r:id="rId22"/>
   <tableParts count="1">
-    <tablePart r:id="rId19"/>
+    <tablePart r:id="rId23"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Javier to list
</commit_message>
<xml_diff>
--- a/CMQA/Organization/RCL-B-CMQA1 Spring 2014 Rascal Personnel Budget.xlsx
+++ b/CMQA/Organization/RCL-B-CMQA1 Spring 2014 Rascal Personnel Budget.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="1305" windowWidth="15480" windowHeight="11640" activeTab="3"/>
+    <workbookView xWindow="2100" yWindow="1305" windowWidth="15480" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="Team Assignments" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="155">
   <si>
     <t>Lead</t>
   </si>
@@ -470,7 +470,22 @@
     <t>Alec Herzog</t>
   </si>
   <si>
-    <t>Javier Delmundo</t>
+    <t>Meeting Times</t>
+  </si>
+  <si>
+    <t>Friday, 5:00 PM</t>
+  </si>
+  <si>
+    <t>Javier Muro De Nadal</t>
+  </si>
+  <si>
+    <t>Muro de Nadal</t>
+  </si>
+  <si>
+    <t>Javier</t>
+  </si>
+  <si>
+    <t>murodenadal@slu.edu</t>
   </si>
 </sst>
 </file>
@@ -517,6 +532,7 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -530,6 +546,7 @@
       <u/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1172,7 +1189,7 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Master Contact Info'!$A$35:$A$39</c:f>
+              <c:f>'Master Contact Info'!$A$36:$A$40</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1195,12 +1212,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Master Contact Info'!$B$35:$B$39</c:f>
+              <c:f>'Master Contact Info'!$B$36:$B$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3</c:v>
@@ -1218,25 +1235,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="67261568"/>
-        <c:axId val="67263104"/>
+        <c:axId val="64351232"/>
+        <c:axId val="66663552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="67261568"/>
+        <c:axId val="64351232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67263104"/>
+        <c:crossAx val="66663552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="67263104"/>
+        <c:axId val="66663552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1262,7 +1278,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67261568"/>
+        <c:crossAx val="64351232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1287,7 +1303,7 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Master Contact Info'!$A$42:$A$48</c:f>
+              <c:f>'Master Contact Info'!$A$43:$A$49</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -1316,7 +1332,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Master Contact Info'!$B$42:$B$48</c:f>
+              <c:f>'Master Contact Info'!$B$43:$B$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1330,7 +1346,7 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>3</c:v>
@@ -1345,25 +1361,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="67381888"/>
-        <c:axId val="67383680"/>
+        <c:axId val="67014016"/>
+        <c:axId val="67044480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="67381888"/>
+        <c:axId val="67014016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67383680"/>
+        <c:crossAx val="67044480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="67383680"/>
+        <c:axId val="67044480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1389,7 +1404,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67381888"/>
+        <c:crossAx val="67014016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1477,8 +1492,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H26" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" headerRowCellStyle="Check Cell">
-  <autoFilter ref="A1:H26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H27" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" headerRowCellStyle="Check Cell">
+  <autoFilter ref="A1:H27"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Last Name" dataDxfId="7"/>
     <tableColumn id="2" name="First Name" dataDxfId="6"/>
@@ -1783,8 +1798,8 @@
   </sheetPr>
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" thickTop="1" thickBottom="1"/>
@@ -1792,7 +1807,7 @@
     <col min="1" max="1" width="10.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
@@ -1917,7 +1932,7 @@
       </c>
       <c r="C7" s="28"/>
       <c r="D7" s="28" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E7" s="28" t="s">
         <v>123</v>
@@ -2019,10 +2034,56 @@
       <c r="H13" s="28"/>
       <c r="I13" s="28"/>
     </row>
-    <row r="14" spans="1:10"/>
-    <row r="15" spans="1:10"/>
-    <row r="16" spans="1:10"/>
-    <row r="17" ht="15"/>
+    <row r="14" spans="1:10" thickTop="1" thickBot="1">
+      <c r="B14" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" thickTop="1" thickBot="1">
+      <c r="B15" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="I15" s="29" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" thickTop="1" thickBot="1">
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+    </row>
     <row r="18" ht="15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2035,10 +2096,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G26" activeCellId="8" sqref="G2 G10 G11 G13 G18 G19 G21 G24 G26"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2417,64 +2478,64 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="14" t="s">
-        <v>16</v>
+        <v>152</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>48</v>
+        <v>153</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>38</v>
+        <v>27</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>53</v>
       </c>
       <c r="F15" s="31" t="s">
-        <v>104</v>
-      </c>
-      <c r="G15" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="H15" s="27" t="s">
-        <v>35</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="G15" s="47" t="s">
+        <v>154</v>
+      </c>
+      <c r="H15" s="13"/>
       <c r="I15" s="12"/>
       <c r="J15" s="11"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="14" t="s">
-        <v>141</v>
+        <v>16</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>142</v>
+        <v>48</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>26</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>53</v>
+        <v>12</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>38</v>
       </c>
       <c r="F16" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="G16" s="46" t="s">
-        <v>143</v>
-      </c>
-      <c r="H16" s="13"/>
+      <c r="G16" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16" s="27" t="s">
+        <v>35</v>
+      </c>
       <c r="I16" s="12"/>
       <c r="J16" s="11"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="14" t="s">
-        <v>112</v>
+        <v>141</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>26</v>
@@ -2486,10 +2547,10 @@
         <v>53</v>
       </c>
       <c r="F17" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="G17" s="32" t="s">
-        <v>113</v>
+        <v>104</v>
+      </c>
+      <c r="G17" s="46" t="s">
+        <v>143</v>
       </c>
       <c r="H17" s="13"/>
       <c r="I17" s="12"/>
@@ -2497,240 +2558,256 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="14" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>85</v>
+        <v>111</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>26</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="F18" s="31" t="s">
-        <v>107</v>
+        <v>70</v>
       </c>
       <c r="G18" s="32" t="s">
-        <v>87</v>
+        <v>113</v>
       </c>
       <c r="H18" s="13"/>
       <c r="I18" s="12"/>
       <c r="J18" s="11"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="23" t="s">
+      <c r="A19" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="24" t="s">
+      <c r="D19" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="10" t="s">
         <v>46</v>
       </c>
       <c r="F19" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="G19" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="H19" s="24"/>
-      <c r="I19" s="9"/>
+        <v>107</v>
+      </c>
+      <c r="G19" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="H19" s="13"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="11"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="22" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="C20" s="23" t="s">
         <v>26</v>
       </c>
       <c r="D20" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="G20" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="H20" s="24"/>
+      <c r="I20" s="9"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="24" t="s">
+      <c r="E21" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="F20" s="31" t="s">
+      <c r="F21" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="G20" s="32" t="s">
+      <c r="G21" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="H20" s="24" t="s">
+      <c r="H21" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="I20" s="9"/>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F21" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="G21" s="47" t="s">
-        <v>146</v>
-      </c>
-      <c r="H21" s="13"/>
       <c r="I21" s="9"/>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="14" t="s">
-        <v>15</v>
+        <v>137</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>72</v>
+        <v>114</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>26</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F22" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="G22" s="32" t="s">
-        <v>73</v>
+        <v>103</v>
+      </c>
+      <c r="G22" s="47" t="s">
+        <v>146</v>
       </c>
       <c r="H22" s="13"/>
       <c r="I22" s="9"/>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="14" t="s">
-        <v>136</v>
+        <v>15</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>135</v>
+        <v>72</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="F23" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="G23" s="47" t="s">
-        <v>147</v>
+        <v>70</v>
+      </c>
+      <c r="G23" s="32" t="s">
+        <v>73</v>
       </c>
       <c r="H23" s="13"/>
       <c r="I23" s="9"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F24" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" s="47" t="s">
+        <v>147</v>
+      </c>
+      <c r="H24" s="13"/>
+      <c r="I24" s="9"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="B24" s="23" t="s">
+      <c r="B25" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="23" t="s">
+      <c r="C25" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="23" t="s">
+      <c r="D25" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="E24" s="24" t="s">
+      <c r="E25" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="F24" s="31" t="s">
+      <c r="F25" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="G24" s="32" t="s">
+      <c r="G25" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="H24" s="24"/>
-      <c r="I24" s="9"/>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="14" t="s">
+      <c r="H25" s="24"/>
+      <c r="I25" s="9"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B26" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C26" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D26" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E26" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F25" s="31" t="s">
+      <c r="F26" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="G25" s="32" t="s">
+      <c r="G26" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="H25" s="13"/>
-      <c r="I25" s="9"/>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="19" t="s">
+      <c r="H26" s="13"/>
+      <c r="I26" s="9"/>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="B27" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="20" t="s">
+      <c r="C27" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D26" s="20" t="s">
+      <c r="D27" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="E26" s="21" t="s">
+      <c r="E27" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="F26" s="38" t="s">
+      <c r="F27" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="G26" s="39" t="s">
+      <c r="G27" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="H26" s="21"/>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27" s="40"/>
-      <c r="B27" s="40"/>
-      <c r="C27" s="40"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="40"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="43"/>
+      <c r="H27" s="21"/>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="40"/>
@@ -2739,16 +2816,12 @@
       <c r="D28" s="40"/>
       <c r="E28" s="40"/>
       <c r="F28" s="41"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="40"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="43"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="44" t="s">
-        <v>91</v>
-      </c>
-      <c r="B29" s="44" t="s">
-        <v>92</v>
-      </c>
+      <c r="A29" s="40"/>
+      <c r="B29" s="40"/>
       <c r="C29" s="40"/>
       <c r="D29" s="40"/>
       <c r="E29" s="40"/>
@@ -2757,12 +2830,11 @@
       <c r="H29" s="40"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B30" s="23">
-        <f t="array" ref="B30">SUM(IF(C2:C26="AE",1,0))</f>
-        <v>21</v>
+      <c r="A30" s="44" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30" s="44" t="s">
+        <v>92</v>
       </c>
       <c r="C30" s="40"/>
       <c r="D30" s="40"/>
@@ -2773,11 +2845,11 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B31" s="23">
-        <f t="array" ref="B31">SUM(IF(C2:C26="EE",1,0))</f>
-        <v>3</v>
+        <f t="array" ref="B31">SUM(IF(C2:C27="AE",1,0))</f>
+        <v>22</v>
       </c>
       <c r="C31" s="40"/>
       <c r="D31" s="40"/>
@@ -2788,10 +2860,11 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="10" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B32" s="23">
-        <v>1</v>
+        <f t="array" ref="B32">SUM(IF(C2:C27="EE",1,0))</f>
+        <v>3</v>
       </c>
       <c r="C32" s="40"/>
       <c r="D32" s="40"/>
@@ -2801,8 +2874,12 @@
       <c r="H32" s="40"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="40"/>
-      <c r="B33" s="40"/>
+      <c r="A33" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="23">
+        <v>1</v>
+      </c>
       <c r="C33" s="40"/>
       <c r="D33" s="40"/>
       <c r="E33" s="40"/>
@@ -2811,12 +2888,8 @@
       <c r="H33" s="40"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="44" t="s">
-        <v>93</v>
-      </c>
-      <c r="B34" s="44" t="s">
-        <v>94</v>
-      </c>
+      <c r="A34" s="40"/>
+      <c r="B34" s="40"/>
       <c r="C34" s="40"/>
       <c r="D34" s="40"/>
       <c r="E34" s="40"/>
@@ -2825,12 +2898,11 @@
       <c r="H34" s="40"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B35" s="23">
-        <f t="array" ref="B35">SUM(IF(D2:D26="Freshman",1,0))</f>
-        <v>8</v>
+      <c r="A35" s="44" t="s">
+        <v>93</v>
+      </c>
+      <c r="B35" s="44" t="s">
+        <v>94</v>
       </c>
       <c r="C35" s="40"/>
       <c r="D35" s="40"/>
@@ -2841,11 +2913,11 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="10" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B36" s="23">
-        <f t="array" ref="B36">SUM(IF(D2:D26="Sophomore",1,0))</f>
-        <v>3</v>
+        <f t="array" ref="B36">SUM(IF(D2:D27="Freshman",1,0))</f>
+        <v>9</v>
       </c>
       <c r="C36" s="40"/>
       <c r="D36" s="40"/>
@@ -2855,24 +2927,27 @@
       <c r="H36" s="40"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B37" s="1">
-        <f t="array" ref="B37">SUM(IF(D2:D26="Junior",1,0))</f>
-        <v>4</v>
-      </c>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="G37" s="11"/>
+      <c r="A37" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" s="23">
+        <f t="array" ref="B37">SUM(IF(D2:D27="Sophomore",1,0))</f>
+        <v>3</v>
+      </c>
+      <c r="C37" s="40"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="40"/>
+      <c r="F37" s="41"/>
+      <c r="G37" s="30"/>
+      <c r="H37" s="40"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B38" s="1">
-        <f t="array" ref="B38">SUM(IF(D2:D26="Senior",1,0))</f>
-        <v>8</v>
+        <f t="array" ref="B38">SUM(IF(D2:D27="Junior",1,0))</f>
+        <v>4</v>
       </c>
       <c r="D38" s="11"/>
       <c r="E38" s="11"/>
@@ -2880,79 +2955,79 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" s="1">
+        <f t="array" ref="B39">SUM(IF(D2:D27="Senior",1,0))</f>
+        <v>8</v>
+      </c>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="G39" s="11"/>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B39" s="1">
-        <f t="array" ref="B39">SUM(IF(D2:D26="Graduate",1,0))</f>
+      <c r="B40" s="1">
+        <f t="array" ref="B40">SUM(IF(D2:D27="Graduate",1,0))</f>
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
-      <c r="A41" s="44" t="s">
+    <row r="42" spans="1:8">
+      <c r="A42" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="B41" s="44" t="s">
+      <c r="B42" s="44" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="42" spans="1:8">
-      <c r="A42" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B42" s="1">
-        <f t="array" ref="B42">SUM(IF(ISNUMBER(SEARCH(A42,$F$2:$F$26)),1,0))</f>
-        <v>1</v>
-      </c>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="G42" s="11"/>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
       <c r="B43" s="1">
-        <f t="array" ref="B43">SUM(IF(ISNUMBER(SEARCH(A43,$F$2:$F$26)),1,0))</f>
-        <v>9</v>
-      </c>
+        <f t="array" ref="B43">SUM(IF(ISNUMBER(SEARCH(A43,$F$2:$F$27)),1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="G43" s="11"/>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
       <c r="B44" s="1">
-        <f t="array" ref="B44">SUM(IF(ISNUMBER(SEARCH(A44,$F$2:$F$26)),1,0))</f>
-        <v>6</v>
+        <f t="array" ref="B44">SUM(IF(ISNUMBER(SEARCH(A44,$F$2:$F$27)),1,0))</f>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="B45" s="1">
-        <f t="array" ref="B45">SUM(IF(ISNUMBER(SEARCH(A45,$F$2:$F$26)),1,0))</f>
-        <v>2</v>
+        <f t="array" ref="B45">SUM(IF(ISNUMBER(SEARCH(A45,$F$2:$F$27)),1,0))</f>
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
-        <v>5</v>
+        <v>86</v>
       </c>
       <c r="B46" s="1">
-        <f t="array" ref="B46">SUM(IF(ISNUMBER(SEARCH(A46,$F$2:$F$26)),1,0))</f>
+        <f t="array" ref="B46">SUM(IF(ISNUMBER(SEARCH(A46,$F$2:$F$27)),1,0))</f>
         <v>3</v>
       </c>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11"/>
-      <c r="G46" s="11"/>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
-        <v>99</v>
+        <v>5</v>
       </c>
       <c r="B47" s="1">
-        <f t="array" ref="B47">SUM(IF(ISNUMBER(SEARCH(A47,$F$2:$F$26)),1,0))</f>
-        <v>6</v>
+        <f t="array" ref="B47">SUM(IF(ISNUMBER(SEARCH(A47,$F$2:$F$27)),1,0))</f>
+        <v>3</v>
       </c>
       <c r="D47" s="11"/>
       <c r="E47" s="11"/>
@@ -2960,53 +3035,66 @@
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B48" s="1">
-        <f t="array" ref="B48">SUM(IF(ISNUMBER(SEARCH(A48,$F$2:$F$26)),1,0))</f>
-        <v>5</v>
+        <f t="array" ref="B48">SUM(IF(ISNUMBER(SEARCH(A48,$F$2:$F$27)),1,0))</f>
+        <v>6</v>
       </c>
       <c r="D48" s="11"/>
       <c r="E48" s="11"/>
       <c r="G48" s="11"/>
     </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="45" t="s">
+    <row r="49" spans="1:7">
+      <c r="A49" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B49" s="1">
+        <f t="array" ref="B49">SUM(IF(ISNUMBER(SEARCH(A49,$F$2:$F$27)),1,0))</f>
+        <v>5</v>
+      </c>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+      <c r="G49" s="11"/>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="B49" s="45">
-        <f t="array" ref="B49">SUM(IF(ISNUMBER(SEARCH(A49,$F$2:$F$26)),1,0))</f>
+      <c r="B50" s="45">
+        <f t="array" ref="B50">SUM(IF(ISNUMBER(SEARCH(A50,$F$2:$F$27)),1,0))</f>
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G3" r:id="rId1"/>
-    <hyperlink ref="G19" r:id="rId2"/>
-    <hyperlink ref="G26" r:id="rId3"/>
+    <hyperlink ref="G20" r:id="rId2"/>
+    <hyperlink ref="G27" r:id="rId3"/>
     <hyperlink ref="G13" r:id="rId4"/>
     <hyperlink ref="G5" r:id="rId5"/>
     <hyperlink ref="G10" r:id="rId6"/>
-    <hyperlink ref="G24" r:id="rId7"/>
+    <hyperlink ref="G25" r:id="rId7"/>
     <hyperlink ref="G8" r:id="rId8"/>
-    <hyperlink ref="G22" r:id="rId9"/>
+    <hyperlink ref="G23" r:id="rId9"/>
     <hyperlink ref="G9" r:id="rId10"/>
     <hyperlink ref="G6" r:id="rId11"/>
-    <hyperlink ref="G18" r:id="rId12"/>
-    <hyperlink ref="G25" r:id="rId13"/>
+    <hyperlink ref="G19" r:id="rId12"/>
+    <hyperlink ref="G26" r:id="rId13"/>
     <hyperlink ref="G11" r:id="rId14"/>
     <hyperlink ref="G7" r:id="rId15"/>
-    <hyperlink ref="G17" r:id="rId16"/>
+    <hyperlink ref="G18" r:id="rId16"/>
     <hyperlink ref="G4" r:id="rId17" display="mailto:nbossart@slu.edu"/>
     <hyperlink ref="G12" r:id="rId18" display="mailto:jmayer16@slu.edu"/>
-    <hyperlink ref="G21" r:id="rId19" display="mailto:sarber@slu.edu"/>
-    <hyperlink ref="G23" r:id="rId20" display="mailto:rurberge@slu.edu"/>
+    <hyperlink ref="G22" r:id="rId19" display="mailto:sarber@slu.edu"/>
+    <hyperlink ref="G24" r:id="rId20" display="mailto:rurberge@slu.edu"/>
     <hyperlink ref="G2" r:id="rId21"/>
+    <hyperlink ref="G15" r:id="rId22" display="mailto:murodenadal@slu.edu"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="78" orientation="landscape" r:id="rId22"/>
+  <pageSetup scale="78" orientation="landscape" r:id="rId23"/>
   <tableParts count="1">
-    <tablePart r:id="rId23"/>
+    <tablePart r:id="rId24"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>